<commit_message>
Grabbed new XLS files from dropbox
</commit_message>
<xml_diff>
--- a/datafiles-2017/xlsfiles/armslength2012to2016_cdc.xlsx
+++ b/datafiles-2017/xlsfiles/armslength2012to2016_cdc.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20700" windowHeight="11760"/>
+    <workbookView xWindow="-420" yWindow="3135" windowWidth="19440" windowHeight="9720"/>
   </bookViews>
   <sheets>
-    <sheet name="armslength" sheetId="1" r:id="rId1"/>
+    <sheet name="Armslength" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="armslength">armslength!$A$1:$CN$31</definedName>
+    <definedName name="Armslength">Armslength!$A$1:$CN$31</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -759,7 +759,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:92" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1105,46 +1105,46 @@
         <v>0</v>
       </c>
       <c r="V2">
-        <v>29250</v>
+        <v>30566</v>
       </c>
       <c r="W2">
-        <v>31000</v>
+        <v>31899</v>
       </c>
       <c r="X2">
-        <v>35000</v>
+        <v>35455</v>
       </c>
       <c r="Y2">
-        <v>42500</v>
+        <v>43095</v>
       </c>
       <c r="Z2">
         <v>46000</v>
       </c>
       <c r="AA2">
-        <v>28750</v>
+        <v>30044</v>
       </c>
       <c r="AB2">
-        <v>30740</v>
+        <v>31631</v>
       </c>
       <c r="AC2">
-        <v>35000</v>
+        <v>35455</v>
       </c>
       <c r="AD2">
-        <v>42000</v>
+        <v>42588</v>
       </c>
       <c r="AE2">
         <v>45400</v>
       </c>
       <c r="AF2">
-        <v>29750</v>
+        <v>31089</v>
       </c>
       <c r="AG2">
-        <v>34500</v>
+        <v>35501</v>
       </c>
       <c r="AH2">
-        <v>40500</v>
+        <v>41027</v>
       </c>
       <c r="AI2">
-        <v>59450</v>
+        <v>60282</v>
       </c>
       <c r="AJ2">
         <v>54500</v>
@@ -1192,13 +1192,13 @@
         <v>-45.53</v>
       </c>
       <c r="BE2">
-        <v>57.26</v>
+        <v>50.49</v>
       </c>
       <c r="BF2">
-        <v>57.91</v>
+        <v>51.11</v>
       </c>
       <c r="BG2">
-        <v>83.19</v>
+        <v>75.3</v>
       </c>
       <c r="BI2">
         <v>134</v>
@@ -1216,16 +1216,16 @@
         <v>254</v>
       </c>
       <c r="BN2">
-        <v>38650</v>
+        <v>40389</v>
       </c>
       <c r="BO2">
-        <v>45600</v>
+        <v>46922</v>
       </c>
       <c r="BP2">
-        <v>42283.5</v>
+        <v>42833</v>
       </c>
       <c r="BQ2">
-        <v>51317.5</v>
+        <v>52036</v>
       </c>
       <c r="BR2">
         <v>50000</v>
@@ -1234,7 +1234,7 @@
         <v>27</v>
       </c>
       <c r="BT2">
-        <v>29.37</v>
+        <v>23.8</v>
       </c>
       <c r="BU2">
         <v>93.33</v>
@@ -1362,61 +1362,61 @@
         <v>37</v>
       </c>
       <c r="V3">
-        <v>14105.5</v>
+        <v>14740</v>
       </c>
       <c r="W3">
-        <v>19118</v>
+        <v>19672</v>
       </c>
       <c r="X3">
-        <v>18013</v>
+        <v>18247</v>
       </c>
       <c r="Y3">
-        <v>22500</v>
+        <v>22815</v>
       </c>
       <c r="Z3">
         <v>22000</v>
       </c>
       <c r="AA3">
-        <v>13000</v>
+        <v>13585</v>
       </c>
       <c r="AB3">
-        <v>21504.5</v>
+        <v>22128</v>
       </c>
       <c r="AC3">
-        <v>19750</v>
+        <v>20007</v>
       </c>
       <c r="AD3">
-        <v>19925</v>
+        <v>20204</v>
       </c>
       <c r="AE3">
         <v>23644.5</v>
       </c>
       <c r="AF3">
-        <v>10000</v>
+        <v>10450</v>
       </c>
       <c r="AG3">
-        <v>8200</v>
+        <v>8438</v>
       </c>
       <c r="AH3">
-        <v>10750</v>
+        <v>10890</v>
       </c>
       <c r="AI3">
-        <v>19400</v>
+        <v>19672</v>
       </c>
       <c r="AJ3">
         <v>10755.5</v>
       </c>
       <c r="AK3">
-        <v>55000</v>
+        <v>57475</v>
       </c>
       <c r="AL3">
-        <v>65000</v>
+        <v>66885</v>
       </c>
       <c r="AM3">
-        <v>65250</v>
+        <v>66098</v>
       </c>
       <c r="AN3">
-        <v>79000</v>
+        <v>80106</v>
       </c>
       <c r="AO3">
         <v>71000</v>
@@ -1467,16 +1467,16 @@
         <v>-21.28</v>
       </c>
       <c r="BE3">
-        <v>55.97</v>
+        <v>49.25</v>
       </c>
       <c r="BF3">
-        <v>81.88</v>
+        <v>74.05</v>
       </c>
       <c r="BG3">
-        <v>7.56</v>
+        <v>2.92</v>
       </c>
       <c r="BH3">
-        <v>29.09</v>
+        <v>23.53</v>
       </c>
       <c r="BI3">
         <v>79</v>
@@ -1494,16 +1494,16 @@
         <v>128</v>
       </c>
       <c r="BN3">
-        <v>20000</v>
+        <v>20900</v>
       </c>
       <c r="BO3">
-        <v>29000</v>
+        <v>29841</v>
       </c>
       <c r="BP3">
-        <v>23525</v>
+        <v>23831</v>
       </c>
       <c r="BQ3">
-        <v>32500</v>
+        <v>32955</v>
       </c>
       <c r="BR3">
         <v>29000</v>
@@ -1512,7 +1512,7 @@
         <v>-0.3</v>
       </c>
       <c r="BT3">
-        <v>45</v>
+        <v>38.76</v>
       </c>
       <c r="BU3">
         <v>44</v>
@@ -1640,58 +1640,58 @@
         <v>3</v>
       </c>
       <c r="V4">
-        <v>16150</v>
+        <v>16877</v>
       </c>
       <c r="W4">
-        <v>25000</v>
+        <v>25725</v>
       </c>
       <c r="X4">
-        <v>30500</v>
+        <v>30897</v>
       </c>
       <c r="Y4">
-        <v>19490</v>
+        <v>19763</v>
       </c>
       <c r="Z4">
         <v>27475</v>
       </c>
       <c r="AA4">
-        <v>26500</v>
+        <v>27693</v>
       </c>
       <c r="AB4">
-        <v>25750</v>
+        <v>26497</v>
       </c>
       <c r="AC4">
-        <v>45028</v>
+        <v>45613</v>
       </c>
       <c r="AD4">
-        <v>30750</v>
+        <v>31181</v>
       </c>
       <c r="AE4">
         <v>29450</v>
       </c>
       <c r="AF4">
-        <v>6300</v>
+        <v>6584</v>
       </c>
       <c r="AG4">
-        <v>4800</v>
+        <v>4939</v>
       </c>
       <c r="AH4">
-        <v>9500</v>
+        <v>9624</v>
       </c>
       <c r="AI4">
-        <v>7371</v>
+        <v>7474</v>
       </c>
       <c r="AJ4">
         <v>16050</v>
       </c>
       <c r="AL4">
-        <v>1820</v>
+        <v>1873</v>
       </c>
       <c r="AM4">
-        <v>6000</v>
+        <v>6078</v>
       </c>
       <c r="AN4">
-        <v>6740</v>
+        <v>6834</v>
       </c>
       <c r="AO4">
         <v>252500</v>
@@ -1739,13 +1739,13 @@
         <v>-57.64</v>
       </c>
       <c r="BE4">
-        <v>70.12</v>
+        <v>62.8</v>
       </c>
       <c r="BF4">
-        <v>11.13</v>
+        <v>6.34</v>
       </c>
       <c r="BG4">
-        <v>154.76</v>
+        <v>143.77000000000001</v>
       </c>
       <c r="BI4">
         <v>15</v>
@@ -1763,16 +1763,16 @@
         <v>35</v>
       </c>
       <c r="BN4">
-        <v>11750</v>
+        <v>12279</v>
       </c>
       <c r="BO4">
-        <v>20200</v>
+        <v>20786</v>
       </c>
       <c r="BP4">
-        <v>36889</v>
+        <v>37369</v>
       </c>
       <c r="BQ4">
-        <v>15000</v>
+        <v>15210</v>
       </c>
       <c r="BR4">
         <v>19900</v>
@@ -1781,7 +1781,7 @@
         <v>64.7</v>
       </c>
       <c r="BT4">
-        <v>69.36</v>
+        <v>62.07</v>
       </c>
       <c r="BU4">
         <v>75</v>
@@ -1909,10 +1909,10 @@
         <v>3</v>
       </c>
       <c r="X5">
-        <v>160000</v>
+        <v>162080</v>
       </c>
       <c r="Y5">
-        <v>206000</v>
+        <v>208884</v>
       </c>
       <c r="Z5">
         <v>231250</v>
@@ -1921,10 +1921,10 @@
         <v>8000</v>
       </c>
       <c r="AM5">
-        <v>160000</v>
+        <v>162080</v>
       </c>
       <c r="AN5">
-        <v>206000</v>
+        <v>208884</v>
       </c>
       <c r="AO5">
         <v>252500</v>
@@ -1969,10 +1969,10 @@
         <v>4</v>
       </c>
       <c r="BP5">
-        <v>160000</v>
+        <v>162080</v>
       </c>
       <c r="BQ5">
-        <v>206000</v>
+        <v>208884</v>
       </c>
       <c r="BR5">
         <v>231250</v>
@@ -2079,46 +2079,46 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <v>12000</v>
+        <v>12540</v>
       </c>
       <c r="W6">
-        <v>15500</v>
+        <v>15950</v>
       </c>
       <c r="X6">
-        <v>17750</v>
+        <v>17981</v>
       </c>
       <c r="Y6">
-        <v>17000</v>
+        <v>17238</v>
       </c>
       <c r="Z6">
         <v>18000</v>
       </c>
       <c r="AA6">
-        <v>13000</v>
+        <v>13585</v>
       </c>
       <c r="AB6">
-        <v>15500</v>
+        <v>15950</v>
       </c>
       <c r="AC6">
-        <v>17500</v>
+        <v>17728</v>
       </c>
       <c r="AD6">
-        <v>17000</v>
+        <v>17238</v>
       </c>
       <c r="AE6">
         <v>16550</v>
       </c>
       <c r="AF6">
-        <v>7750</v>
+        <v>8099</v>
       </c>
       <c r="AG6">
-        <v>14950</v>
+        <v>15384</v>
       </c>
       <c r="AH6">
-        <v>18000</v>
+        <v>18234</v>
       </c>
       <c r="AI6">
-        <v>18076</v>
+        <v>18329</v>
       </c>
       <c r="AJ6">
         <v>19900</v>
@@ -2166,13 +2166,13 @@
         <v>-36.020000000000003</v>
       </c>
       <c r="BE6">
-        <v>50</v>
+        <v>43.54</v>
       </c>
       <c r="BF6">
-        <v>27.31</v>
+        <v>21.83</v>
       </c>
       <c r="BG6">
-        <v>156.77000000000001</v>
+        <v>145.71</v>
       </c>
       <c r="BI6">
         <v>16</v>
@@ -2190,16 +2190,16 @@
         <v>42</v>
       </c>
       <c r="BN6">
-        <v>16000</v>
+        <v>16720</v>
       </c>
       <c r="BO6">
-        <v>17500</v>
+        <v>18008</v>
       </c>
       <c r="BP6">
-        <v>17500</v>
+        <v>17728</v>
       </c>
       <c r="BQ6">
-        <v>22917.5</v>
+        <v>23238</v>
       </c>
       <c r="BR6">
         <v>19859.5</v>
@@ -2208,7 +2208,7 @@
         <v>72.760000000000005</v>
       </c>
       <c r="BT6">
-        <v>24.12</v>
+        <v>18.78</v>
       </c>
       <c r="BU6">
         <v>61.04</v>
@@ -2336,61 +2336,61 @@
         <v>12</v>
       </c>
       <c r="V7">
-        <v>20550</v>
+        <v>21475</v>
       </c>
       <c r="W7">
-        <v>26750</v>
+        <v>27526</v>
       </c>
       <c r="X7">
-        <v>30000</v>
+        <v>30390</v>
       </c>
       <c r="Y7">
-        <v>31950</v>
+        <v>32397</v>
       </c>
       <c r="Z7">
         <v>37500</v>
       </c>
       <c r="AA7">
-        <v>26000</v>
+        <v>27170</v>
       </c>
       <c r="AB7">
-        <v>22900</v>
+        <v>23564</v>
       </c>
       <c r="AC7">
-        <v>30000</v>
+        <v>30390</v>
       </c>
       <c r="AD7">
-        <v>26000</v>
+        <v>26364</v>
       </c>
       <c r="AE7">
         <v>32100</v>
       </c>
       <c r="AF7">
-        <v>16306.5</v>
+        <v>17040</v>
       </c>
       <c r="AG7">
-        <v>30000</v>
+        <v>30870</v>
       </c>
       <c r="AH7">
-        <v>28700</v>
+        <v>29073</v>
       </c>
       <c r="AI7">
-        <v>37300</v>
+        <v>37822</v>
       </c>
       <c r="AJ7">
         <v>40000</v>
       </c>
       <c r="AK7">
-        <v>56500</v>
+        <v>59043</v>
       </c>
       <c r="AL7">
-        <v>44000</v>
+        <v>45276</v>
       </c>
       <c r="AM7">
-        <v>44250</v>
+        <v>44825</v>
       </c>
       <c r="AN7">
-        <v>48500</v>
+        <v>49179</v>
       </c>
       <c r="AO7">
         <v>67750</v>
@@ -2441,16 +2441,16 @@
         <v>-32.97</v>
       </c>
       <c r="BE7">
-        <v>82.48</v>
+        <v>74.62</v>
       </c>
       <c r="BF7">
-        <v>23.46</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="BG7">
-        <v>145.30000000000001</v>
+        <v>134.74</v>
       </c>
       <c r="BH7">
-        <v>19.91</v>
+        <v>14.75</v>
       </c>
       <c r="BI7">
         <v>67</v>
@@ -2468,16 +2468,16 @@
         <v>111</v>
       </c>
       <c r="BN7">
-        <v>38000</v>
+        <v>39710</v>
       </c>
       <c r="BO7">
-        <v>40000</v>
+        <v>41160</v>
       </c>
       <c r="BP7">
-        <v>40900</v>
+        <v>41432</v>
       </c>
       <c r="BQ7">
-        <v>50000</v>
+        <v>50700</v>
       </c>
       <c r="BR7">
         <v>47300</v>
@@ -2486,7 +2486,7 @@
         <v>-1.99</v>
       </c>
       <c r="BT7">
-        <v>24.47</v>
+        <v>19.11</v>
       </c>
       <c r="BU7">
         <v>64.290000000000006</v>
@@ -2614,61 +2614,61 @@
         <v>23</v>
       </c>
       <c r="V8">
-        <v>27500</v>
+        <v>28738</v>
       </c>
       <c r="W8">
-        <v>29150</v>
+        <v>29995</v>
       </c>
       <c r="X8">
-        <v>37900</v>
+        <v>38393</v>
       </c>
       <c r="Y8">
-        <v>40000</v>
+        <v>40560</v>
       </c>
       <c r="Z8">
         <v>75000</v>
       </c>
       <c r="AA8">
-        <v>22900</v>
+        <v>23931</v>
       </c>
       <c r="AB8">
-        <v>25925</v>
+        <v>26677</v>
       </c>
       <c r="AC8">
-        <v>38000</v>
+        <v>38494</v>
       </c>
       <c r="AD8">
-        <v>33100</v>
+        <v>33563</v>
       </c>
       <c r="AE8">
         <v>88000</v>
       </c>
       <c r="AF8">
-        <v>40000</v>
+        <v>41800</v>
       </c>
       <c r="AG8">
-        <v>20000</v>
+        <v>20580</v>
       </c>
       <c r="AH8">
-        <v>24750</v>
+        <v>25072</v>
       </c>
       <c r="AI8">
-        <v>35000</v>
+        <v>35490</v>
       </c>
       <c r="AJ8">
         <v>40375</v>
       </c>
       <c r="AK8">
-        <v>252000</v>
+        <v>263340</v>
       </c>
       <c r="AL8">
-        <v>205000</v>
+        <v>210945</v>
       </c>
       <c r="AM8">
-        <v>234720</v>
+        <v>237771</v>
       </c>
       <c r="AN8">
-        <v>155412.5</v>
+        <v>157588</v>
       </c>
       <c r="AO8">
         <v>285000</v>
@@ -2719,16 +2719,16 @@
         <v>-54.92</v>
       </c>
       <c r="BE8">
-        <v>172.73</v>
+        <v>160.97999999999999</v>
       </c>
       <c r="BF8">
-        <v>284.27999999999997</v>
+        <v>267.72000000000003</v>
       </c>
       <c r="BG8">
-        <v>0.94</v>
+        <v>-3.41</v>
       </c>
       <c r="BH8">
-        <v>13.1</v>
+        <v>8.23</v>
       </c>
       <c r="BI8">
         <v>64</v>
@@ -2746,16 +2746,16 @@
         <v>148</v>
       </c>
       <c r="BN8">
-        <v>43750</v>
+        <v>45719</v>
       </c>
       <c r="BO8">
-        <v>57900</v>
+        <v>59579</v>
       </c>
       <c r="BP8">
-        <v>45000</v>
+        <v>45585</v>
       </c>
       <c r="BQ8">
-        <v>50000</v>
+        <v>50700</v>
       </c>
       <c r="BR8">
         <v>98500</v>
@@ -2764,7 +2764,7 @@
         <v>21.56</v>
       </c>
       <c r="BT8">
-        <v>125.14</v>
+        <v>115.45</v>
       </c>
       <c r="BU8">
         <v>67.48</v>
@@ -2892,46 +2892,46 @@
         <v>68</v>
       </c>
       <c r="V9">
-        <v>202000</v>
+        <v>211090</v>
       </c>
       <c r="W9">
-        <v>230000</v>
+        <v>236670</v>
       </c>
       <c r="X9">
-        <v>200000</v>
+        <v>202600</v>
       </c>
       <c r="Y9">
-        <v>190000</v>
+        <v>192660</v>
       </c>
       <c r="Z9">
         <v>182000</v>
       </c>
       <c r="AA9">
-        <v>307000</v>
+        <v>320815</v>
       </c>
       <c r="AB9">
-        <v>287719</v>
+        <v>296063</v>
       </c>
       <c r="AC9">
-        <v>336500</v>
+        <v>340875</v>
       </c>
       <c r="AD9">
-        <v>275000</v>
+        <v>278850</v>
       </c>
       <c r="AE9">
         <v>273000</v>
       </c>
       <c r="AK9">
-        <v>200000</v>
+        <v>209000</v>
       </c>
       <c r="AL9">
-        <v>202500</v>
+        <v>208373</v>
       </c>
       <c r="AM9">
-        <v>199000</v>
+        <v>201587</v>
       </c>
       <c r="AN9">
-        <v>190000</v>
+        <v>192660</v>
       </c>
       <c r="AO9">
         <v>181000</v>
@@ -2976,13 +2976,13 @@
         <v>1.21</v>
       </c>
       <c r="BE9">
-        <v>-9.9</v>
+        <v>-13.78</v>
       </c>
       <c r="BF9">
-        <v>-11.07</v>
+        <v>-14.9</v>
       </c>
       <c r="BH9">
-        <v>-9.5</v>
+        <v>-13.4</v>
       </c>
       <c r="BI9">
         <v>36</v>
@@ -3000,16 +3000,16 @@
         <v>67</v>
       </c>
       <c r="BN9">
-        <v>204500</v>
+        <v>213703</v>
       </c>
       <c r="BO9">
-        <v>234250</v>
+        <v>241043</v>
       </c>
       <c r="BP9">
-        <v>200000</v>
+        <v>202600</v>
       </c>
       <c r="BQ9">
-        <v>190000</v>
+        <v>192660</v>
       </c>
       <c r="BR9">
         <v>182000</v>
@@ -3018,7 +3018,7 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="BT9">
-        <v>-11</v>
+        <v>-14.84</v>
       </c>
       <c r="BU9">
         <v>2.63</v>
@@ -3146,46 +3146,46 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <v>10050</v>
+        <v>10502</v>
       </c>
       <c r="W10">
-        <v>15875</v>
+        <v>16335</v>
       </c>
       <c r="X10">
-        <v>22500</v>
+        <v>22793</v>
       </c>
       <c r="Y10">
-        <v>36200</v>
+        <v>36707</v>
       </c>
       <c r="Z10">
         <v>23200</v>
       </c>
       <c r="AA10">
-        <v>16800</v>
+        <v>17556</v>
       </c>
       <c r="AB10">
-        <v>31750</v>
+        <v>32671</v>
       </c>
       <c r="AC10">
-        <v>47250</v>
+        <v>47864</v>
       </c>
       <c r="AD10">
-        <v>60000</v>
+        <v>60840</v>
       </c>
       <c r="AE10">
         <v>32000</v>
       </c>
       <c r="AF10">
-        <v>6250</v>
+        <v>6531</v>
       </c>
       <c r="AG10">
-        <v>3750</v>
+        <v>3859</v>
       </c>
       <c r="AH10">
-        <v>5100</v>
+        <v>5166</v>
       </c>
       <c r="AI10">
-        <v>9500</v>
+        <v>9633</v>
       </c>
       <c r="AJ10">
         <v>14200</v>
@@ -3233,13 +3233,13 @@
         <v>-39.14</v>
       </c>
       <c r="BE10">
-        <v>130.85</v>
+        <v>120.91</v>
       </c>
       <c r="BF10">
-        <v>90.48</v>
+        <v>82.27</v>
       </c>
       <c r="BG10">
-        <v>127.2</v>
+        <v>117.42</v>
       </c>
       <c r="BI10">
         <v>16</v>
@@ -3257,16 +3257,16 @@
         <v>36</v>
       </c>
       <c r="BN10">
-        <v>54500</v>
+        <v>56953</v>
       </c>
       <c r="BO10">
-        <v>32500</v>
+        <v>33443</v>
       </c>
       <c r="BP10">
-        <v>14800</v>
+        <v>14992</v>
       </c>
       <c r="BQ10">
-        <v>16250</v>
+        <v>16478</v>
       </c>
       <c r="BR10">
         <v>23125</v>
@@ -3275,7 +3275,7 @@
         <v>50</v>
       </c>
       <c r="BT10">
-        <v>-57.57</v>
+        <v>-59.4</v>
       </c>
       <c r="BU10">
         <v>65.22</v>
@@ -3403,58 +3403,58 @@
         <v>1</v>
       </c>
       <c r="V11">
-        <v>13000</v>
+        <v>13585</v>
       </c>
       <c r="W11">
-        <v>10000</v>
+        <v>10290</v>
       </c>
       <c r="X11">
-        <v>16619</v>
+        <v>16835</v>
       </c>
       <c r="Y11">
-        <v>17675</v>
+        <v>17922</v>
       </c>
       <c r="Z11">
         <v>16000</v>
       </c>
       <c r="AA11">
-        <v>11750</v>
+        <v>12279</v>
       </c>
       <c r="AB11">
-        <v>11900</v>
+        <v>12245</v>
       </c>
       <c r="AC11">
-        <v>19000</v>
+        <v>19247</v>
       </c>
       <c r="AD11">
-        <v>17150</v>
+        <v>17390</v>
       </c>
       <c r="AE11">
         <v>16900</v>
       </c>
       <c r="AF11">
-        <v>14000</v>
+        <v>14630</v>
       </c>
       <c r="AG11">
-        <v>9500</v>
+        <v>9776</v>
       </c>
       <c r="AH11">
-        <v>14400</v>
+        <v>14587</v>
       </c>
       <c r="AI11">
-        <v>18250</v>
+        <v>18506</v>
       </c>
       <c r="AJ11">
         <v>15000</v>
       </c>
       <c r="AL11">
-        <v>1000</v>
+        <v>1029</v>
       </c>
       <c r="AM11">
-        <v>3000</v>
+        <v>3039</v>
       </c>
       <c r="AN11">
-        <v>85000</v>
+        <v>86190</v>
       </c>
       <c r="AO11">
         <v>14325</v>
@@ -3502,13 +3502,13 @@
         <v>-23.6</v>
       </c>
       <c r="BE11">
-        <v>23.08</v>
+        <v>17.78</v>
       </c>
       <c r="BF11">
-        <v>43.83</v>
+        <v>37.630000000000003</v>
       </c>
       <c r="BG11">
-        <v>7.14</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="BI11">
         <v>78</v>
@@ -3526,16 +3526,16 @@
         <v>151</v>
       </c>
       <c r="BN11">
-        <v>16100</v>
+        <v>16825</v>
       </c>
       <c r="BO11">
-        <v>15800</v>
+        <v>16258</v>
       </c>
       <c r="BP11">
-        <v>23650</v>
+        <v>23957</v>
       </c>
       <c r="BQ11">
-        <v>20000</v>
+        <v>20280</v>
       </c>
       <c r="BR11">
         <v>21700</v>
@@ -3544,7 +3544,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="BT11">
-        <v>34.78</v>
+        <v>28.97</v>
       </c>
       <c r="BU11">
         <v>56.41</v>
@@ -3672,31 +3672,31 @@
         <v>35</v>
       </c>
       <c r="V12">
-        <v>205000</v>
+        <v>214225</v>
       </c>
       <c r="W12">
-        <v>162000</v>
+        <v>166698</v>
       </c>
       <c r="X12">
-        <v>200000</v>
+        <v>202600</v>
       </c>
       <c r="Y12">
-        <v>179500</v>
+        <v>182013</v>
       </c>
       <c r="Z12">
         <v>165500</v>
       </c>
       <c r="AK12">
-        <v>205000</v>
+        <v>214225</v>
       </c>
       <c r="AL12">
-        <v>162000</v>
+        <v>166698</v>
       </c>
       <c r="AM12">
-        <v>200000</v>
+        <v>202600</v>
       </c>
       <c r="AN12">
-        <v>179500</v>
+        <v>182013</v>
       </c>
       <c r="AO12">
         <v>165500</v>
@@ -3738,10 +3738,10 @@
         <v>0</v>
       </c>
       <c r="BE12">
-        <v>-19.27</v>
+        <v>-22.74</v>
       </c>
       <c r="BH12">
-        <v>-19.27</v>
+        <v>-22.74</v>
       </c>
       <c r="BI12">
         <v>14</v>
@@ -3759,16 +3759,16 @@
         <v>33</v>
       </c>
       <c r="BN12">
-        <v>223000</v>
+        <v>233035</v>
       </c>
       <c r="BO12">
-        <v>200000</v>
+        <v>205800</v>
       </c>
       <c r="BP12">
-        <v>200000</v>
+        <v>202600</v>
       </c>
       <c r="BQ12">
-        <v>175000</v>
+        <v>177450</v>
       </c>
       <c r="BR12">
         <v>165500</v>
@@ -3777,7 +3777,7 @@
         <v>1.03</v>
       </c>
       <c r="BT12">
-        <v>-25.78</v>
+        <v>-28.98</v>
       </c>
       <c r="BU12">
         <v>0</v>
@@ -3905,46 +3905,46 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>16250</v>
+        <v>16981</v>
       </c>
       <c r="W13">
-        <v>18900</v>
+        <v>19448</v>
       </c>
       <c r="X13">
-        <v>19200</v>
+        <v>19450</v>
       </c>
       <c r="Y13">
-        <v>21667</v>
+        <v>21970</v>
       </c>
       <c r="Z13">
         <v>24750</v>
       </c>
       <c r="AA13">
-        <v>17100</v>
+        <v>17870</v>
       </c>
       <c r="AB13">
-        <v>19000</v>
+        <v>19551</v>
       </c>
       <c r="AC13">
-        <v>19100</v>
+        <v>19348</v>
       </c>
       <c r="AD13">
-        <v>22000</v>
+        <v>22308</v>
       </c>
       <c r="AE13">
         <v>25000</v>
       </c>
       <c r="AF13">
-        <v>9750</v>
+        <v>10189</v>
       </c>
       <c r="AG13">
-        <v>16233.5</v>
+        <v>16704</v>
       </c>
       <c r="AH13">
-        <v>19500</v>
+        <v>19754</v>
       </c>
       <c r="AI13">
-        <v>20000</v>
+        <v>20280</v>
       </c>
       <c r="AJ13">
         <v>22000</v>
@@ -3992,13 +3992,13 @@
         <v>-25.73</v>
       </c>
       <c r="BE13">
-        <v>52.31</v>
+        <v>45.75</v>
       </c>
       <c r="BF13">
-        <v>46.2</v>
+        <v>39.9</v>
       </c>
       <c r="BG13">
-        <v>125.64</v>
+        <v>115.92</v>
       </c>
       <c r="BI13">
         <v>84</v>
@@ -4016,16 +4016,16 @@
         <v>172</v>
       </c>
       <c r="BN13">
-        <v>22900</v>
+        <v>23931</v>
       </c>
       <c r="BO13">
-        <v>22900</v>
+        <v>23564</v>
       </c>
       <c r="BP13">
-        <v>22000</v>
+        <v>22286</v>
       </c>
       <c r="BQ13">
-        <v>24000</v>
+        <v>24336</v>
       </c>
       <c r="BR13">
         <v>24419</v>
@@ -4034,7 +4034,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="BT13">
-        <v>6.63</v>
+        <v>2.04</v>
       </c>
       <c r="BU13">
         <v>90.63</v>
@@ -4162,31 +4162,31 @@
         <v>7</v>
       </c>
       <c r="V14">
-        <v>152000</v>
+        <v>158840</v>
       </c>
       <c r="W14">
-        <v>216250</v>
+        <v>222521</v>
       </c>
       <c r="X14">
-        <v>168350</v>
+        <v>170539</v>
       </c>
       <c r="Y14">
-        <v>345950.5</v>
+        <v>350794</v>
       </c>
       <c r="Z14">
         <v>180000</v>
       </c>
       <c r="AK14">
-        <v>152000</v>
+        <v>158840</v>
       </c>
       <c r="AL14">
-        <v>216250</v>
+        <v>222521</v>
       </c>
       <c r="AM14">
-        <v>168350</v>
+        <v>170539</v>
       </c>
       <c r="AN14">
-        <v>345950.5</v>
+        <v>350794</v>
       </c>
       <c r="AO14">
         <v>180000</v>
@@ -4228,10 +4228,10 @@
         <v>0</v>
       </c>
       <c r="BE14">
-        <v>18.420000000000002</v>
+        <v>13.32</v>
       </c>
       <c r="BH14">
-        <v>18.420000000000002</v>
+        <v>13.32</v>
       </c>
       <c r="BI14">
         <v>5</v>
@@ -4249,16 +4249,16 @@
         <v>7</v>
       </c>
       <c r="BN14">
-        <v>152000</v>
+        <v>158840</v>
       </c>
       <c r="BO14">
-        <v>216250</v>
+        <v>222521</v>
       </c>
       <c r="BP14">
-        <v>160000</v>
+        <v>162080</v>
       </c>
       <c r="BQ14">
-        <v>331901</v>
+        <v>336548</v>
       </c>
       <c r="BR14">
         <v>180000</v>
@@ -4267,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="BT14">
-        <v>18.420000000000002</v>
+        <v>13.32</v>
       </c>
       <c r="BU14">
         <v>0</v>
@@ -4395,37 +4395,37 @@
         <v>25</v>
       </c>
       <c r="V15">
-        <v>187400</v>
+        <v>195833</v>
       </c>
       <c r="W15">
-        <v>230000</v>
+        <v>236670</v>
       </c>
       <c r="X15">
-        <v>174900</v>
+        <v>177174</v>
       </c>
       <c r="Y15">
-        <v>190000</v>
+        <v>192660</v>
       </c>
       <c r="Z15">
         <v>197500</v>
       </c>
       <c r="AC15">
-        <v>336500</v>
+        <v>340875</v>
       </c>
       <c r="AD15">
-        <v>365000</v>
+        <v>370110</v>
       </c>
       <c r="AK15">
-        <v>187400</v>
+        <v>195833</v>
       </c>
       <c r="AL15">
-        <v>230000</v>
+        <v>236670</v>
       </c>
       <c r="AM15">
-        <v>174000</v>
+        <v>176262</v>
       </c>
       <c r="AN15">
-        <v>185000</v>
+        <v>187590</v>
       </c>
       <c r="AO15">
         <v>197500</v>
@@ -4467,10 +4467,10 @@
         <v>0</v>
       </c>
       <c r="BE15">
-        <v>5.39</v>
+        <v>0.85</v>
       </c>
       <c r="BH15">
-        <v>5.39</v>
+        <v>0.85</v>
       </c>
       <c r="BI15">
         <v>17</v>
@@ -4488,16 +4488,16 @@
         <v>25</v>
       </c>
       <c r="BN15">
-        <v>188000</v>
+        <v>196460</v>
       </c>
       <c r="BO15">
-        <v>230000</v>
+        <v>236670</v>
       </c>
       <c r="BP15">
-        <v>174900</v>
+        <v>177174</v>
       </c>
       <c r="BQ15">
-        <v>195000</v>
+        <v>197730</v>
       </c>
       <c r="BR15">
         <v>197500</v>
@@ -4506,7 +4506,7 @@
         <v>5.89</v>
       </c>
       <c r="BT15">
-        <v>5.05</v>
+        <v>0.53</v>
       </c>
       <c r="BU15">
         <v>0</v>
@@ -4634,58 +4634,58 @@
         <v>0</v>
       </c>
       <c r="V16">
-        <v>12250</v>
+        <v>12801</v>
       </c>
       <c r="W16">
-        <v>15600</v>
+        <v>16052</v>
       </c>
       <c r="X16">
-        <v>13650</v>
+        <v>13827</v>
       </c>
       <c r="Y16">
-        <v>12100</v>
+        <v>12269</v>
       </c>
       <c r="Z16">
         <v>16200</v>
       </c>
       <c r="AA16">
-        <v>16025</v>
+        <v>16746</v>
       </c>
       <c r="AB16">
-        <v>17900</v>
+        <v>18419</v>
       </c>
       <c r="AC16">
-        <v>14500</v>
+        <v>14689</v>
       </c>
       <c r="AD16">
-        <v>10977.5</v>
+        <v>11131</v>
       </c>
       <c r="AE16">
         <v>15000</v>
       </c>
       <c r="AF16">
-        <v>8625</v>
+        <v>9013</v>
       </c>
       <c r="AG16">
-        <v>9577.5</v>
+        <v>9855</v>
       </c>
       <c r="AH16">
-        <v>12825</v>
+        <v>12992</v>
       </c>
       <c r="AI16">
-        <v>12900</v>
+        <v>13081</v>
       </c>
       <c r="AJ16">
         <v>18500</v>
       </c>
       <c r="AK16">
-        <v>105000</v>
+        <v>109725</v>
       </c>
       <c r="AL16">
-        <v>85000</v>
+        <v>87465</v>
       </c>
       <c r="AN16">
-        <v>160000</v>
+        <v>162240</v>
       </c>
       <c r="AP16">
         <v>48</v>
@@ -4733,13 +4733,13 @@
         <v>-17.760000000000002</v>
       </c>
       <c r="BE16">
-        <v>32.24</v>
+        <v>26.55</v>
       </c>
       <c r="BF16">
-        <v>-6.4</v>
+        <v>-10.43</v>
       </c>
       <c r="BG16">
-        <v>114.49</v>
+        <v>105.26</v>
       </c>
       <c r="BI16">
         <v>43</v>
@@ -4757,16 +4757,16 @@
         <v>79</v>
       </c>
       <c r="BN16">
-        <v>20000</v>
+        <v>20900</v>
       </c>
       <c r="BO16">
-        <v>20300</v>
+        <v>20889</v>
       </c>
       <c r="BP16">
-        <v>15000</v>
+        <v>15195</v>
       </c>
       <c r="BQ16">
-        <v>15000</v>
+        <v>15210</v>
       </c>
       <c r="BR16">
         <v>19800</v>
@@ -4775,7 +4775,7 @@
         <v>34.29</v>
       </c>
       <c r="BT16">
-        <v>-1</v>
+        <v>-5.26</v>
       </c>
       <c r="BU16">
         <v>61.32</v>
@@ -4903,61 +4903,61 @@
         <v>1</v>
       </c>
       <c r="V17">
-        <v>77000</v>
+        <v>80465</v>
       </c>
       <c r="W17">
-        <v>87450</v>
+        <v>89986</v>
       </c>
       <c r="X17">
-        <v>93000</v>
+        <v>94209</v>
       </c>
       <c r="Y17">
-        <v>94000</v>
+        <v>95316</v>
       </c>
       <c r="Z17">
         <v>104000</v>
       </c>
       <c r="AA17">
-        <v>77000</v>
+        <v>80465</v>
       </c>
       <c r="AB17">
-        <v>87500</v>
+        <v>90038</v>
       </c>
       <c r="AC17">
-        <v>92500</v>
+        <v>93703</v>
       </c>
       <c r="AD17">
-        <v>93000</v>
+        <v>94302</v>
       </c>
       <c r="AE17">
         <v>103500</v>
       </c>
       <c r="AF17">
-        <v>81700</v>
+        <v>85377</v>
       </c>
       <c r="AG17">
-        <v>80137.5</v>
+        <v>82461</v>
       </c>
       <c r="AH17">
-        <v>117250</v>
+        <v>118774</v>
       </c>
       <c r="AI17">
-        <v>118543.5</v>
+        <v>120203</v>
       </c>
       <c r="AJ17">
         <v>121975</v>
       </c>
       <c r="AK17">
-        <v>12700</v>
+        <v>13272</v>
       </c>
       <c r="AL17">
-        <v>25000</v>
+        <v>25725</v>
       </c>
       <c r="AM17">
-        <v>45000</v>
+        <v>45585</v>
       </c>
       <c r="AN17">
-        <v>99500</v>
+        <v>100893</v>
       </c>
       <c r="AO17">
         <v>14000</v>
@@ -5008,16 +5008,16 @@
         <v>-60.4</v>
       </c>
       <c r="BE17">
-        <v>35.06</v>
+        <v>29.25</v>
       </c>
       <c r="BF17">
-        <v>34.42</v>
+        <v>28.63</v>
       </c>
       <c r="BG17">
-        <v>49.3</v>
+        <v>42.87</v>
       </c>
       <c r="BH17">
-        <v>10.24</v>
+        <v>5.49</v>
       </c>
       <c r="BI17">
         <v>206</v>
@@ -5035,16 +5035,16 @@
         <v>396</v>
       </c>
       <c r="BN17">
-        <v>83500</v>
+        <v>87258</v>
       </c>
       <c r="BO17">
-        <v>95500</v>
+        <v>98270</v>
       </c>
       <c r="BP17">
-        <v>97200</v>
+        <v>98464</v>
       </c>
       <c r="BQ17">
-        <v>99500</v>
+        <v>100893</v>
       </c>
       <c r="BR17">
         <v>109450</v>
@@ -5053,7 +5053,7 @@
         <v>13.81</v>
       </c>
       <c r="BT17">
-        <v>31.08</v>
+        <v>25.43</v>
       </c>
       <c r="BU17">
         <v>96.62</v>
@@ -5181,61 +5181,61 @@
         <v>5</v>
       </c>
       <c r="V18">
-        <v>188750</v>
+        <v>197244</v>
       </c>
       <c r="W18">
-        <v>185000</v>
+        <v>190365</v>
       </c>
       <c r="X18">
-        <v>195000</v>
+        <v>197535</v>
       </c>
       <c r="Y18">
-        <v>209950</v>
+        <v>212889</v>
       </c>
       <c r="Z18">
         <v>180000</v>
       </c>
       <c r="AA18">
-        <v>455000</v>
+        <v>475475</v>
       </c>
       <c r="AB18">
-        <v>380000</v>
+        <v>391020</v>
       </c>
       <c r="AC18">
-        <v>385000</v>
+        <v>390005</v>
       </c>
       <c r="AD18">
-        <v>324500</v>
+        <v>329043</v>
       </c>
       <c r="AE18">
         <v>461250</v>
       </c>
       <c r="AF18">
-        <v>158000</v>
+        <v>165110</v>
       </c>
       <c r="AG18">
-        <v>125000</v>
+        <v>128625</v>
       </c>
       <c r="AH18">
-        <v>156750</v>
+        <v>158788</v>
       </c>
       <c r="AI18">
-        <v>158000</v>
+        <v>160212</v>
       </c>
       <c r="AJ18">
         <v>158000</v>
       </c>
       <c r="AK18">
-        <v>129900</v>
+        <v>135746</v>
       </c>
       <c r="AL18">
-        <v>330000</v>
+        <v>339570</v>
       </c>
       <c r="AM18">
-        <v>383750</v>
+        <v>388739</v>
       </c>
       <c r="AN18">
-        <v>173000</v>
+        <v>175422</v>
       </c>
       <c r="AO18">
         <v>161500</v>
@@ -5283,16 +5283,16 @@
         <v>-16.670000000000002</v>
       </c>
       <c r="BE18">
-        <v>-4.6399999999999997</v>
+        <v>-8.74</v>
       </c>
       <c r="BF18">
-        <v>1.37</v>
+        <v>-2.99</v>
       </c>
       <c r="BG18">
-        <v>0</v>
+        <v>-4.3099999999999996</v>
       </c>
       <c r="BH18">
-        <v>24.33</v>
+        <v>18.97</v>
       </c>
       <c r="BI18">
         <v>8</v>
@@ -5310,16 +5310,16 @@
         <v>16</v>
       </c>
       <c r="BN18">
-        <v>188750</v>
+        <v>197244</v>
       </c>
       <c r="BO18">
-        <v>257500</v>
+        <v>264968</v>
       </c>
       <c r="BP18">
-        <v>195000</v>
+        <v>197535</v>
       </c>
       <c r="BQ18">
-        <v>209950</v>
+        <v>212889</v>
       </c>
       <c r="BR18">
         <v>180000</v>
@@ -5328,7 +5328,7 @@
         <v>0</v>
       </c>
       <c r="BT18">
-        <v>-4.6399999999999997</v>
+        <v>-8.74</v>
       </c>
       <c r="BU18">
         <v>37.5</v>
@@ -5456,46 +5456,46 @@
         <v>0</v>
       </c>
       <c r="V19">
-        <v>12000</v>
+        <v>12540</v>
       </c>
       <c r="W19">
-        <v>15000</v>
+        <v>15435</v>
       </c>
       <c r="X19">
-        <v>19912</v>
+        <v>20171</v>
       </c>
       <c r="Y19">
-        <v>18250</v>
+        <v>18506</v>
       </c>
       <c r="Z19">
         <v>20000</v>
       </c>
       <c r="AA19">
-        <v>12000</v>
+        <v>12540</v>
       </c>
       <c r="AB19">
-        <v>15000</v>
+        <v>15435</v>
       </c>
       <c r="AC19">
-        <v>19725</v>
+        <v>19981</v>
       </c>
       <c r="AD19">
-        <v>17800</v>
+        <v>18049</v>
       </c>
       <c r="AE19">
         <v>18888</v>
       </c>
       <c r="AF19">
-        <v>12250</v>
+        <v>12801</v>
       </c>
       <c r="AG19">
-        <v>14500</v>
+        <v>14921</v>
       </c>
       <c r="AH19">
-        <v>22000</v>
+        <v>22286</v>
       </c>
       <c r="AI19">
-        <v>19200</v>
+        <v>19469</v>
       </c>
       <c r="AJ19">
         <v>24500</v>
@@ -5543,13 +5543,13 @@
         <v>-43.14</v>
       </c>
       <c r="BE19">
-        <v>66.67</v>
+        <v>59.49</v>
       </c>
       <c r="BF19">
-        <v>57.4</v>
+        <v>50.62</v>
       </c>
       <c r="BG19">
-        <v>100</v>
+        <v>91.39</v>
       </c>
       <c r="BI19">
         <v>138</v>
@@ -5567,16 +5567,16 @@
         <v>199</v>
       </c>
       <c r="BN19">
-        <v>14050</v>
+        <v>14682</v>
       </c>
       <c r="BO19">
-        <v>17921</v>
+        <v>18441</v>
       </c>
       <c r="BP19">
-        <v>22500</v>
+        <v>22793</v>
       </c>
       <c r="BQ19">
-        <v>20000</v>
+        <v>20280</v>
       </c>
       <c r="BR19">
         <v>24000</v>
@@ -5585,7 +5585,7 @@
         <v>-2.75</v>
       </c>
       <c r="BT19">
-        <v>70.819999999999993</v>
+        <v>63.47</v>
       </c>
       <c r="BU19">
         <v>66.900000000000006</v>
@@ -5713,55 +5713,55 @@
         <v>0</v>
       </c>
       <c r="V20">
-        <v>69500</v>
+        <v>72628</v>
       </c>
       <c r="W20">
-        <v>27500</v>
+        <v>28298</v>
       </c>
       <c r="X20">
-        <v>65000</v>
+        <v>65845</v>
       </c>
       <c r="Y20">
-        <v>115500</v>
+        <v>117117</v>
       </c>
       <c r="Z20">
         <v>61000</v>
       </c>
       <c r="AA20">
-        <v>69500</v>
+        <v>72628</v>
       </c>
       <c r="AB20">
-        <v>22600</v>
+        <v>23255</v>
       </c>
       <c r="AC20">
-        <v>32800</v>
+        <v>33226</v>
       </c>
       <c r="AE20">
         <v>169950</v>
       </c>
       <c r="AF20">
-        <v>52000</v>
+        <v>54340</v>
       </c>
       <c r="AG20">
-        <v>25000</v>
+        <v>25725</v>
       </c>
       <c r="AH20">
-        <v>79000</v>
+        <v>80027</v>
       </c>
       <c r="AI20">
-        <v>51625</v>
+        <v>52348</v>
       </c>
       <c r="AJ20">
         <v>55000</v>
       </c>
       <c r="AK20">
-        <v>105000</v>
+        <v>109725</v>
       </c>
       <c r="AL20">
-        <v>85000</v>
+        <v>87465</v>
       </c>
       <c r="AN20">
-        <v>160000</v>
+        <v>162240</v>
       </c>
       <c r="AP20">
         <v>0</v>
@@ -5806,13 +5806,13 @@
         <v>-100</v>
       </c>
       <c r="BE20">
-        <v>-12.23</v>
+        <v>-16.010000000000002</v>
       </c>
       <c r="BF20">
-        <v>144.53</v>
+        <v>134</v>
       </c>
       <c r="BG20">
-        <v>5.77</v>
+        <v>1.21</v>
       </c>
       <c r="BI20">
         <v>2</v>
@@ -5830,16 +5830,16 @@
         <v>5</v>
       </c>
       <c r="BN20">
-        <v>62500</v>
+        <v>65313</v>
       </c>
       <c r="BO20">
-        <v>27500</v>
+        <v>28298</v>
       </c>
       <c r="BP20">
-        <v>65000</v>
+        <v>65845</v>
       </c>
       <c r="BQ20">
-        <v>115500</v>
+        <v>117117</v>
       </c>
       <c r="BR20">
         <v>61000</v>
@@ -5848,7 +5848,7 @@
         <v>100</v>
       </c>
       <c r="BT20">
-        <v>-2.4</v>
+        <v>-6.6</v>
       </c>
       <c r="BU20">
         <v>50</v>
@@ -5976,46 +5976,46 @@
         <v>0</v>
       </c>
       <c r="V21">
-        <v>8525</v>
+        <v>8909</v>
       </c>
       <c r="W21">
-        <v>12000</v>
+        <v>12348</v>
       </c>
       <c r="X21">
-        <v>12642</v>
+        <v>12806</v>
       </c>
       <c r="Y21">
-        <v>14700</v>
+        <v>14906</v>
       </c>
       <c r="Z21">
         <v>13500</v>
       </c>
       <c r="AA21">
-        <v>9000</v>
+        <v>9405</v>
       </c>
       <c r="AB21">
-        <v>10062</v>
+        <v>10354</v>
       </c>
       <c r="AC21">
-        <v>11850</v>
+        <v>12004</v>
       </c>
       <c r="AD21">
-        <v>17150</v>
+        <v>17390</v>
       </c>
       <c r="AE21">
         <v>12615.5</v>
       </c>
       <c r="AF21">
-        <v>7000</v>
+        <v>7315</v>
       </c>
       <c r="AG21">
-        <v>17000</v>
+        <v>17493</v>
       </c>
       <c r="AH21">
-        <v>12642</v>
+        <v>12806</v>
       </c>
       <c r="AI21">
-        <v>11000</v>
+        <v>11154</v>
       </c>
       <c r="AJ21">
         <v>14000</v>
@@ -6063,13 +6063,13 @@
         <v>-35.299999999999997</v>
       </c>
       <c r="BE21">
-        <v>58.36</v>
+        <v>51.53</v>
       </c>
       <c r="BF21">
-        <v>40.17</v>
+        <v>34.14</v>
       </c>
       <c r="BG21">
-        <v>100</v>
+        <v>91.39</v>
       </c>
       <c r="BI21">
         <v>52</v>
@@ -6087,16 +6087,16 @@
         <v>98</v>
       </c>
       <c r="BN21">
-        <v>11000</v>
+        <v>11495</v>
       </c>
       <c r="BO21">
-        <v>18000</v>
+        <v>18522</v>
       </c>
       <c r="BP21">
-        <v>17290</v>
+        <v>17515</v>
       </c>
       <c r="BQ21">
-        <v>23000</v>
+        <v>23322</v>
       </c>
       <c r="BR21">
         <v>17000</v>
@@ -6105,7 +6105,7 @@
         <v>-6.07</v>
       </c>
       <c r="BT21">
-        <v>54.55</v>
+        <v>47.89</v>
       </c>
       <c r="BU21">
         <v>62.35</v>
@@ -6233,58 +6233,58 @@
         <v>0</v>
       </c>
       <c r="V22">
-        <v>25500</v>
+        <v>26648</v>
       </c>
       <c r="W22">
-        <v>28900</v>
+        <v>29738</v>
       </c>
       <c r="X22">
-        <v>32500</v>
+        <v>32923</v>
       </c>
       <c r="Y22">
-        <v>35000</v>
+        <v>35490</v>
       </c>
       <c r="Z22">
         <v>34000</v>
       </c>
       <c r="AA22">
-        <v>26000</v>
+        <v>27170</v>
       </c>
       <c r="AB22">
-        <v>30332</v>
+        <v>31212</v>
       </c>
       <c r="AC22">
-        <v>33400</v>
+        <v>33834</v>
       </c>
       <c r="AD22">
-        <v>37500</v>
+        <v>38025</v>
       </c>
       <c r="AE22">
         <v>38850</v>
       </c>
       <c r="AF22">
-        <v>24000</v>
+        <v>25080</v>
       </c>
       <c r="AG22">
-        <v>26500</v>
+        <v>27269</v>
       </c>
       <c r="AH22">
-        <v>29500</v>
+        <v>29884</v>
       </c>
       <c r="AI22">
-        <v>25800</v>
+        <v>26161</v>
       </c>
       <c r="AJ22">
         <v>22500</v>
       </c>
       <c r="AK22">
-        <v>53750</v>
+        <v>56169</v>
       </c>
       <c r="AM22">
-        <v>119900</v>
+        <v>121459</v>
       </c>
       <c r="AN22">
-        <v>159000</v>
+        <v>161226</v>
       </c>
       <c r="AP22">
         <v>34</v>
@@ -6332,13 +6332,13 @@
         <v>-22.46</v>
       </c>
       <c r="BE22">
-        <v>33.33</v>
+        <v>27.59</v>
       </c>
       <c r="BF22">
-        <v>49.42</v>
+        <v>42.99</v>
       </c>
       <c r="BG22">
-        <v>-6.25</v>
+        <v>-10.29</v>
       </c>
       <c r="BI22">
         <v>89</v>
@@ -6356,16 +6356,16 @@
         <v>112</v>
       </c>
       <c r="BN22">
-        <v>34500</v>
+        <v>36053</v>
       </c>
       <c r="BO22">
-        <v>38000</v>
+        <v>39102</v>
       </c>
       <c r="BP22">
-        <v>40000</v>
+        <v>40520</v>
       </c>
       <c r="BQ22">
-        <v>47000</v>
+        <v>47658</v>
       </c>
       <c r="BR22">
         <v>41375</v>
@@ -6374,7 +6374,7 @@
         <v>-7.82</v>
       </c>
       <c r="BT22">
-        <v>19.93</v>
+        <v>14.76</v>
       </c>
       <c r="BU22">
         <v>71.349999999999994</v>
@@ -6502,61 +6502,61 @@
         <v>11</v>
       </c>
       <c r="V23">
-        <v>120750</v>
+        <v>126184</v>
       </c>
       <c r="W23">
-        <v>65000</v>
+        <v>66885</v>
       </c>
       <c r="X23">
-        <v>130000</v>
+        <v>131690</v>
       </c>
       <c r="Y23">
-        <v>81250</v>
+        <v>82388</v>
       </c>
       <c r="Z23">
         <v>114000</v>
       </c>
       <c r="AA23">
-        <v>80000</v>
+        <v>83600</v>
       </c>
       <c r="AB23">
-        <v>62206</v>
+        <v>64010</v>
       </c>
       <c r="AC23">
-        <v>125000</v>
+        <v>126625</v>
       </c>
       <c r="AD23">
-        <v>95500</v>
+        <v>96837</v>
       </c>
       <c r="AE23">
         <v>107500</v>
       </c>
       <c r="AF23">
-        <v>35000</v>
+        <v>36575</v>
       </c>
       <c r="AG23">
-        <v>29000</v>
+        <v>29841</v>
       </c>
       <c r="AH23">
-        <v>89000</v>
+        <v>90157</v>
       </c>
       <c r="AI23">
-        <v>52500</v>
+        <v>53235</v>
       </c>
       <c r="AJ23">
         <v>90500</v>
       </c>
       <c r="AK23">
-        <v>184250</v>
+        <v>192541</v>
       </c>
       <c r="AL23">
-        <v>207450</v>
+        <v>213466</v>
       </c>
       <c r="AM23">
-        <v>200000</v>
+        <v>202600</v>
       </c>
       <c r="AN23">
-        <v>225000</v>
+        <v>228150</v>
       </c>
       <c r="AO23">
         <v>245000</v>
@@ -6607,16 +6607,16 @@
         <v>-57.65</v>
       </c>
       <c r="BE23">
-        <v>-5.59</v>
+        <v>-9.66</v>
       </c>
       <c r="BF23">
-        <v>34.380000000000003</v>
+        <v>28.59</v>
       </c>
       <c r="BG23">
-        <v>158.57</v>
+        <v>147.44</v>
       </c>
       <c r="BH23">
-        <v>32.97</v>
+        <v>27.25</v>
       </c>
       <c r="BI23">
         <v>60</v>
@@ -6634,16 +6634,16 @@
         <v>93</v>
       </c>
       <c r="BN23">
-        <v>160500</v>
+        <v>167723</v>
       </c>
       <c r="BO23">
-        <v>95000</v>
+        <v>97755</v>
       </c>
       <c r="BP23">
-        <v>147000</v>
+        <v>148911</v>
       </c>
       <c r="BQ23">
-        <v>101900</v>
+        <v>103327</v>
       </c>
       <c r="BR23">
         <v>108000</v>
@@ -6652,7 +6652,7 @@
         <v>-1.48</v>
       </c>
       <c r="BT23">
-        <v>-32.71</v>
+        <v>-35.61</v>
       </c>
       <c r="BU23">
         <v>45.12</v>
@@ -6780,61 +6780,61 @@
         <v>8</v>
       </c>
       <c r="V24">
-        <v>43000</v>
+        <v>44935</v>
       </c>
       <c r="W24">
-        <v>40000</v>
+        <v>41160</v>
       </c>
       <c r="X24">
-        <v>50000</v>
+        <v>50650</v>
       </c>
       <c r="Y24">
-        <v>53000</v>
+        <v>53742</v>
       </c>
       <c r="Z24">
         <v>59000</v>
       </c>
       <c r="AA24">
-        <v>43250</v>
+        <v>45196</v>
       </c>
       <c r="AB24">
-        <v>42150</v>
+        <v>43372</v>
       </c>
       <c r="AC24">
-        <v>51000</v>
+        <v>51663</v>
       </c>
       <c r="AD24">
-        <v>53200</v>
+        <v>53945</v>
       </c>
       <c r="AE24">
         <v>60000</v>
       </c>
       <c r="AF24">
-        <v>38000</v>
+        <v>39710</v>
       </c>
       <c r="AG24">
-        <v>30600</v>
+        <v>31487</v>
       </c>
       <c r="AH24">
-        <v>44000</v>
+        <v>44572</v>
       </c>
       <c r="AI24">
-        <v>46250</v>
+        <v>46898</v>
       </c>
       <c r="AJ24">
         <v>50000</v>
       </c>
       <c r="AK24">
-        <v>50500</v>
+        <v>52773</v>
       </c>
       <c r="AL24">
-        <v>73000</v>
+        <v>75117</v>
       </c>
       <c r="AM24">
-        <v>80000</v>
+        <v>81040</v>
       </c>
       <c r="AN24">
-        <v>84000</v>
+        <v>85176</v>
       </c>
       <c r="AO24">
         <v>78250</v>
@@ -6885,16 +6885,16 @@
         <v>-31.47</v>
       </c>
       <c r="BE24">
-        <v>37.21</v>
+        <v>31.3</v>
       </c>
       <c r="BF24">
-        <v>38.729999999999997</v>
+        <v>32.76</v>
       </c>
       <c r="BG24">
-        <v>31.58</v>
+        <v>25.91</v>
       </c>
       <c r="BH24">
-        <v>54.95</v>
+        <v>48.28</v>
       </c>
       <c r="BI24">
         <v>222</v>
@@ -6912,16 +6912,16 @@
         <v>329</v>
       </c>
       <c r="BN24">
-        <v>56450</v>
+        <v>58990</v>
       </c>
       <c r="BO24">
-        <v>55000</v>
+        <v>56595</v>
       </c>
       <c r="BP24">
-        <v>57420</v>
+        <v>58166</v>
       </c>
       <c r="BQ24">
-        <v>59250</v>
+        <v>60080</v>
       </c>
       <c r="BR24">
         <v>65000</v>
@@ -6930,7 +6930,7 @@
         <v>9.3699999999999992</v>
       </c>
       <c r="BT24">
-        <v>15.15</v>
+        <v>10.19</v>
       </c>
       <c r="BU24">
         <v>83.38</v>
@@ -7058,61 +7058,61 @@
         <v>36</v>
       </c>
       <c r="V25">
-        <v>48500</v>
+        <v>50683</v>
       </c>
       <c r="W25">
-        <v>48750</v>
+        <v>50164</v>
       </c>
       <c r="X25">
-        <v>40500</v>
+        <v>41027</v>
       </c>
       <c r="Y25">
-        <v>59500</v>
+        <v>60333</v>
       </c>
       <c r="Z25">
         <v>57750</v>
       </c>
       <c r="AA25">
-        <v>45000</v>
+        <v>47025</v>
       </c>
       <c r="AB25">
-        <v>28000</v>
+        <v>28812</v>
       </c>
       <c r="AC25">
-        <v>35000</v>
+        <v>35455</v>
       </c>
       <c r="AD25">
-        <v>40650</v>
+        <v>41219</v>
       </c>
       <c r="AE25">
         <v>45500</v>
       </c>
       <c r="AF25">
-        <v>25500</v>
+        <v>26648</v>
       </c>
       <c r="AG25">
-        <v>46000</v>
+        <v>47334</v>
       </c>
       <c r="AH25">
-        <v>24125</v>
+        <v>24439</v>
       </c>
       <c r="AI25">
-        <v>29959</v>
+        <v>30378</v>
       </c>
       <c r="AJ25">
         <v>33750.5</v>
       </c>
       <c r="AK25">
-        <v>61250</v>
+        <v>64006</v>
       </c>
       <c r="AL25">
-        <v>65000</v>
+        <v>66885</v>
       </c>
       <c r="AM25">
-        <v>65250</v>
+        <v>66098</v>
       </c>
       <c r="AN25">
-        <v>79500</v>
+        <v>80613</v>
       </c>
       <c r="AO25">
         <v>72000</v>
@@ -7163,16 +7163,16 @@
         <v>-41.01</v>
       </c>
       <c r="BE25">
-        <v>19.07</v>
+        <v>13.94</v>
       </c>
       <c r="BF25">
-        <v>1.1100000000000001</v>
+        <v>-3.24</v>
       </c>
       <c r="BG25">
-        <v>32.35</v>
+        <v>26.65</v>
       </c>
       <c r="BH25">
-        <v>17.55</v>
+        <v>12.49</v>
       </c>
       <c r="BI25">
         <v>35</v>
@@ -7190,16 +7190,16 @@
         <v>59</v>
       </c>
       <c r="BN25">
-        <v>55000</v>
+        <v>57475</v>
       </c>
       <c r="BO25">
-        <v>65000</v>
+        <v>66885</v>
       </c>
       <c r="BP25">
-        <v>57000</v>
+        <v>57741</v>
       </c>
       <c r="BQ25">
-        <v>76000</v>
+        <v>77064</v>
       </c>
       <c r="BR25">
         <v>69900</v>
@@ -7208,7 +7208,7 @@
         <v>13.6</v>
       </c>
       <c r="BT25">
-        <v>27.09</v>
+        <v>21.62</v>
       </c>
       <c r="BU25">
         <v>50</v>
@@ -7336,46 +7336,46 @@
         <v>0</v>
       </c>
       <c r="V26">
-        <v>12500</v>
+        <v>13063</v>
       </c>
       <c r="W26">
-        <v>12500</v>
+        <v>12863</v>
       </c>
       <c r="X26">
-        <v>15000</v>
+        <v>15195</v>
       </c>
       <c r="Y26">
-        <v>14650</v>
+        <v>14855</v>
       </c>
       <c r="Z26">
         <v>13000</v>
       </c>
       <c r="AA26">
-        <v>12000</v>
+        <v>12540</v>
       </c>
       <c r="AB26">
-        <v>13350</v>
+        <v>13737</v>
       </c>
       <c r="AC26">
-        <v>15750</v>
+        <v>15955</v>
       </c>
       <c r="AD26">
-        <v>14137</v>
+        <v>14335</v>
       </c>
       <c r="AE26">
         <v>14000</v>
       </c>
       <c r="AF26">
-        <v>13350</v>
+        <v>13951</v>
       </c>
       <c r="AG26">
-        <v>10908.5</v>
+        <v>11225</v>
       </c>
       <c r="AH26">
-        <v>12764</v>
+        <v>12930</v>
       </c>
       <c r="AI26">
-        <v>15000</v>
+        <v>15210</v>
       </c>
       <c r="AJ26">
         <v>11500</v>
@@ -7423,13 +7423,13 @@
         <v>1.22</v>
       </c>
       <c r="BE26">
-        <v>4</v>
+        <v>-0.48</v>
       </c>
       <c r="BF26">
-        <v>16.670000000000002</v>
+        <v>11.64</v>
       </c>
       <c r="BG26">
-        <v>-13.86</v>
+        <v>-17.57</v>
       </c>
       <c r="BI26">
         <v>143</v>
@@ -7447,16 +7447,16 @@
         <v>196</v>
       </c>
       <c r="BN26">
-        <v>15000</v>
+        <v>15675</v>
       </c>
       <c r="BO26">
-        <v>17300</v>
+        <v>17802</v>
       </c>
       <c r="BP26">
-        <v>17000</v>
+        <v>17221</v>
       </c>
       <c r="BQ26">
-        <v>15500</v>
+        <v>15717</v>
       </c>
       <c r="BR26">
         <v>17450</v>
@@ -7465,7 +7465,7 @@
         <v>7.39</v>
       </c>
       <c r="BT26">
-        <v>16.329999999999998</v>
+        <v>11.32</v>
       </c>
       <c r="BU26">
         <v>71.430000000000007</v>
@@ -7593,58 +7593,58 @@
         <v>0</v>
       </c>
       <c r="V27">
-        <v>9500</v>
+        <v>9928</v>
       </c>
       <c r="W27">
-        <v>14100</v>
+        <v>14509</v>
       </c>
       <c r="X27">
-        <v>14100</v>
+        <v>14283</v>
       </c>
       <c r="Y27">
-        <v>13811</v>
+        <v>14004</v>
       </c>
       <c r="Z27">
         <v>15000</v>
       </c>
       <c r="AA27">
-        <v>10122</v>
+        <v>10577</v>
       </c>
       <c r="AB27">
-        <v>16500</v>
+        <v>16979</v>
       </c>
       <c r="AC27">
-        <v>14929</v>
+        <v>15123</v>
       </c>
       <c r="AD27">
-        <v>13500</v>
+        <v>13689</v>
       </c>
       <c r="AE27">
         <v>15800</v>
       </c>
       <c r="AF27">
-        <v>8427</v>
+        <v>8806</v>
       </c>
       <c r="AG27">
-        <v>9412</v>
+        <v>9685</v>
       </c>
       <c r="AH27">
-        <v>12500</v>
+        <v>12663</v>
       </c>
       <c r="AI27">
-        <v>14600</v>
+        <v>14804</v>
       </c>
       <c r="AJ27">
         <v>14000</v>
       </c>
       <c r="AL27">
-        <v>85000</v>
+        <v>87465</v>
       </c>
       <c r="AM27">
-        <v>177500</v>
+        <v>179808</v>
       </c>
       <c r="AN27">
-        <v>149000</v>
+        <v>151086</v>
       </c>
       <c r="AP27">
         <v>163</v>
@@ -7689,13 +7689,13 @@
         <v>-27.38</v>
       </c>
       <c r="BE27">
-        <v>57.89</v>
+        <v>51.09</v>
       </c>
       <c r="BF27">
-        <v>56.1</v>
+        <v>49.38</v>
       </c>
       <c r="BG27">
-        <v>66.13</v>
+        <v>58.98</v>
       </c>
       <c r="BI27">
         <v>107</v>
@@ -7713,16 +7713,16 @@
         <v>199</v>
       </c>
       <c r="BN27">
-        <v>15000</v>
+        <v>15675</v>
       </c>
       <c r="BO27">
-        <v>17000</v>
+        <v>17493</v>
       </c>
       <c r="BP27">
-        <v>16600</v>
+        <v>16816</v>
       </c>
       <c r="BQ27">
-        <v>18250</v>
+        <v>18506</v>
       </c>
       <c r="BR27">
         <v>20000</v>
@@ -7731,7 +7731,7 @@
         <v>30.25</v>
       </c>
       <c r="BT27">
-        <v>33.33</v>
+        <v>27.59</v>
       </c>
       <c r="BU27">
         <v>58.84</v>
@@ -7859,61 +7859,61 @@
         <v>4</v>
       </c>
       <c r="V28">
-        <v>84950</v>
+        <v>88773</v>
       </c>
       <c r="W28">
-        <v>110857.5</v>
+        <v>114072</v>
       </c>
       <c r="X28">
-        <v>85000</v>
+        <v>86105</v>
       </c>
       <c r="Y28">
-        <v>87500</v>
+        <v>88725</v>
       </c>
       <c r="Z28">
         <v>90000</v>
       </c>
       <c r="AA28">
-        <v>112000</v>
+        <v>117040</v>
       </c>
       <c r="AB28">
-        <v>128000</v>
+        <v>131712</v>
       </c>
       <c r="AC28">
-        <v>100000</v>
+        <v>101300</v>
       </c>
       <c r="AD28">
-        <v>120000</v>
+        <v>121680</v>
       </c>
       <c r="AE28">
         <v>136000</v>
       </c>
       <c r="AF28">
-        <v>49000</v>
+        <v>51205</v>
       </c>
       <c r="AG28">
-        <v>50000</v>
+        <v>51450</v>
       </c>
       <c r="AH28">
-        <v>62500</v>
+        <v>63313</v>
       </c>
       <c r="AI28">
-        <v>52500</v>
+        <v>53235</v>
       </c>
       <c r="AJ28">
         <v>70000</v>
       </c>
       <c r="AK28">
-        <v>210000</v>
+        <v>219450</v>
       </c>
       <c r="AL28">
-        <v>161500</v>
+        <v>166184</v>
       </c>
       <c r="AM28">
-        <v>173500</v>
+        <v>175756</v>
       </c>
       <c r="AN28">
-        <v>244817.5</v>
+        <v>248245</v>
       </c>
       <c r="AO28">
         <v>152500</v>
@@ -7964,16 +7964,16 @@
         <v>-46.99</v>
       </c>
       <c r="BE28">
-        <v>5.94</v>
+        <v>1.38</v>
       </c>
       <c r="BF28">
-        <v>21.43</v>
+        <v>16.2</v>
       </c>
       <c r="BG28">
-        <v>42.86</v>
+        <v>36.71</v>
       </c>
       <c r="BH28">
-        <v>-27.38</v>
+        <v>-30.51</v>
       </c>
       <c r="BI28">
         <v>65</v>
@@ -7991,16 +7991,16 @@
         <v>97</v>
       </c>
       <c r="BN28">
-        <v>120000</v>
+        <v>125400</v>
       </c>
       <c r="BO28">
-        <v>125000</v>
+        <v>128625</v>
       </c>
       <c r="BP28">
-        <v>97000</v>
+        <v>98261</v>
       </c>
       <c r="BQ28">
-        <v>97500</v>
+        <v>98865</v>
       </c>
       <c r="BR28">
         <v>100000</v>
@@ -8009,7 +8009,7 @@
         <v>8.76</v>
       </c>
       <c r="BT28">
-        <v>-16.670000000000002</v>
+        <v>-20.260000000000002</v>
       </c>
       <c r="BU28">
         <v>67.44</v>
@@ -8137,46 +8137,46 @@
         <v>0</v>
       </c>
       <c r="V29">
-        <v>7910</v>
+        <v>8266</v>
       </c>
       <c r="W29">
-        <v>11000</v>
+        <v>11319</v>
       </c>
       <c r="X29">
-        <v>13833</v>
+        <v>14013</v>
       </c>
       <c r="Y29">
-        <v>14000</v>
+        <v>14196</v>
       </c>
       <c r="Z29">
         <v>12000</v>
       </c>
       <c r="AA29">
-        <v>9354</v>
+        <v>9775</v>
       </c>
       <c r="AB29">
-        <v>12000</v>
+        <v>12348</v>
       </c>
       <c r="AC29">
-        <v>14000</v>
+        <v>14182</v>
       </c>
       <c r="AD29">
-        <v>15000</v>
+        <v>15210</v>
       </c>
       <c r="AE29">
         <v>11019.5</v>
       </c>
       <c r="AF29">
-        <v>5580</v>
+        <v>5831</v>
       </c>
       <c r="AG29">
-        <v>10000</v>
+        <v>10290</v>
       </c>
       <c r="AH29">
-        <v>11500</v>
+        <v>11650</v>
       </c>
       <c r="AI29">
-        <v>10000</v>
+        <v>10140</v>
       </c>
       <c r="AJ29">
         <v>13500</v>
@@ -8224,13 +8224,13 @@
         <v>-22.17</v>
       </c>
       <c r="BE29">
-        <v>51.71</v>
+        <v>45.17</v>
       </c>
       <c r="BF29">
-        <v>17.809999999999999</v>
+        <v>12.73</v>
       </c>
       <c r="BG29">
-        <v>141.94</v>
+        <v>131.52000000000001</v>
       </c>
       <c r="BI29">
         <v>77</v>
@@ -8248,16 +8248,16 @@
         <v>167</v>
       </c>
       <c r="BN29">
-        <v>9000</v>
+        <v>9405</v>
       </c>
       <c r="BO29">
-        <v>16500</v>
+        <v>16979</v>
       </c>
       <c r="BP29">
-        <v>19900</v>
+        <v>20159</v>
       </c>
       <c r="BQ29">
-        <v>18950</v>
+        <v>19215</v>
       </c>
       <c r="BR29">
         <v>16500</v>
@@ -8266,7 +8266,7 @@
         <v>18.55</v>
       </c>
       <c r="BT29">
-        <v>83.33</v>
+        <v>75.44</v>
       </c>
       <c r="BU29">
         <v>72.22</v>
@@ -8394,49 +8394,49 @@
         <v>1</v>
       </c>
       <c r="V30">
-        <v>330061</v>
+        <v>344914</v>
       </c>
       <c r="W30">
-        <v>218000</v>
+        <v>224322</v>
       </c>
       <c r="X30">
-        <v>312500</v>
+        <v>316563</v>
       </c>
       <c r="Y30">
-        <v>65000</v>
+        <v>65910</v>
       </c>
       <c r="Z30">
         <v>97500</v>
       </c>
       <c r="AA30">
-        <v>351622</v>
+        <v>367445</v>
       </c>
       <c r="AB30">
-        <v>349500</v>
+        <v>359636</v>
       </c>
       <c r="AC30">
-        <v>312500</v>
+        <v>316563</v>
       </c>
       <c r="AD30">
-        <v>313500</v>
+        <v>317889</v>
       </c>
       <c r="AE30">
         <v>97500</v>
       </c>
       <c r="AG30">
-        <v>57500</v>
+        <v>59168</v>
       </c>
       <c r="AI30">
-        <v>55000</v>
+        <v>55770</v>
       </c>
       <c r="AK30">
-        <v>32500</v>
+        <v>33963</v>
       </c>
       <c r="AL30">
-        <v>105000</v>
+        <v>108045</v>
       </c>
       <c r="AN30">
-        <v>61899.5</v>
+        <v>62766</v>
       </c>
       <c r="AO30">
         <v>250000</v>
@@ -8481,13 +8481,13 @@
         <v>33.32</v>
       </c>
       <c r="BE30">
-        <v>-70.459999999999994</v>
+        <v>-71.73</v>
       </c>
       <c r="BF30">
-        <v>-72.27</v>
+        <v>-73.47</v>
       </c>
       <c r="BH30">
-        <v>669.23</v>
+        <v>636.1</v>
       </c>
       <c r="BI30">
         <v>3</v>
@@ -8505,16 +8505,16 @@
         <v>2</v>
       </c>
       <c r="BN30">
-        <v>351622</v>
+        <v>367445</v>
       </c>
       <c r="BO30">
-        <v>331000</v>
+        <v>340599</v>
       </c>
       <c r="BP30">
-        <v>312500</v>
+        <v>316563</v>
       </c>
       <c r="BQ30">
-        <v>75000</v>
+        <v>76050</v>
       </c>
       <c r="BR30">
         <v>97500</v>
@@ -8523,7 +8523,7 @@
         <v>-11.11</v>
       </c>
       <c r="BT30">
-        <v>-72.27</v>
+        <v>-73.47</v>
       </c>
       <c r="BU30">
         <v>75</v>
@@ -8651,46 +8651,46 @@
         <v>1</v>
       </c>
       <c r="V31">
-        <v>24500</v>
+        <v>25603</v>
       </c>
       <c r="W31">
-        <v>25000</v>
+        <v>25725</v>
       </c>
       <c r="X31">
-        <v>29000</v>
+        <v>29377</v>
       </c>
       <c r="Y31">
-        <v>28500</v>
+        <v>28899</v>
       </c>
       <c r="Z31">
         <v>35937.5</v>
       </c>
       <c r="AA31">
-        <v>25000</v>
+        <v>26125</v>
       </c>
       <c r="AB31">
-        <v>26000</v>
+        <v>26754</v>
       </c>
       <c r="AC31">
-        <v>28300</v>
+        <v>28668</v>
       </c>
       <c r="AD31">
-        <v>27500</v>
+        <v>27885</v>
       </c>
       <c r="AE31">
         <v>35000</v>
       </c>
       <c r="AF31">
-        <v>24000</v>
+        <v>25080</v>
       </c>
       <c r="AG31">
-        <v>23275</v>
+        <v>23950</v>
       </c>
       <c r="AH31">
-        <v>37000</v>
+        <v>37481</v>
       </c>
       <c r="AI31">
-        <v>39000</v>
+        <v>39546</v>
       </c>
       <c r="AJ31">
         <v>38000</v>
@@ -8741,13 +8741,13 @@
         <v>-16.39</v>
       </c>
       <c r="BE31">
-        <v>46.68</v>
+        <v>40.36</v>
       </c>
       <c r="BF31">
-        <v>40</v>
+        <v>33.97</v>
       </c>
       <c r="BG31">
-        <v>58.33</v>
+        <v>51.52</v>
       </c>
       <c r="BI31">
         <v>96</v>
@@ -8765,16 +8765,16 @@
         <v>179</v>
       </c>
       <c r="BN31">
-        <v>30000</v>
+        <v>31350</v>
       </c>
       <c r="BO31">
-        <v>31175</v>
+        <v>32079</v>
       </c>
       <c r="BP31">
-        <v>33000</v>
+        <v>33429</v>
       </c>
       <c r="BQ31">
-        <v>37550</v>
+        <v>38076</v>
       </c>
       <c r="BR31">
         <v>40000</v>
@@ -8783,7 +8783,7 @@
         <v>18.14</v>
       </c>
       <c r="BT31">
-        <v>33.33</v>
+        <v>27.59</v>
       </c>
       <c r="BU31">
         <v>78.44</v>

</xml_diff>